<commit_message>
adds backlog and sprints
</commit_message>
<xml_diff>
--- a/final+project.xlsx
+++ b/final+project.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="63">
   <si>
     <t>Your Name:</t>
   </si>
@@ -128,9 +128,6 @@
     <t>Will Fergus</t>
   </si>
   <si>
-    <t>I can use it</t>
-  </si>
-  <si>
     <t>I can stop using it</t>
   </si>
   <si>
@@ -143,34 +140,85 @@
     <t>The app works on the device I'm currently using</t>
   </si>
   <si>
-    <t>UI elements</t>
-  </si>
-  <si>
-    <t>I can navigate the app</t>
-  </si>
-  <si>
-    <t>To start the app</t>
-  </si>
-  <si>
-    <t>To quit the app</t>
-  </si>
-  <si>
     <t xml:space="preserve">Cross-platform compatability </t>
   </si>
   <si>
     <t>CrossPlat</t>
   </si>
   <si>
-    <t xml:space="preserve">UI </t>
-  </si>
-  <si>
-    <t>Something to look at on screen</t>
-  </si>
-  <si>
-    <t>For entertainment?</t>
-  </si>
-  <si>
-    <t>LottieDottie</t>
+    <t>For entertainment? Because its pretty?</t>
+  </si>
+  <si>
+    <t>A reason to open the app</t>
+  </si>
+  <si>
+    <t>LottieDottieDa</t>
+  </si>
+  <si>
+    <t>The one and only D. O. double G</t>
+  </si>
+  <si>
+    <t>task</t>
+  </si>
+  <si>
+    <t>I can select an animation</t>
+  </si>
+  <si>
+    <t>Selection buttons</t>
+  </si>
+  <si>
+    <t>UI_Select</t>
+  </si>
+  <si>
+    <t>UI_Back</t>
+  </si>
+  <si>
+    <t>A return/back button</t>
+  </si>
+  <si>
+    <t>I can go back to choosing an animation</t>
+  </si>
+  <si>
+    <t>I can start using it</t>
+  </si>
+  <si>
+    <t>To open the app</t>
+  </si>
+  <si>
+    <t>To exit the app</t>
+  </si>
+  <si>
+    <t>Make sure xamarin is working properly</t>
+  </si>
+  <si>
+    <t>UI_Selection</t>
+  </si>
+  <si>
+    <t>Create buttons that open the corresponding lottie animation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create a back/retrun to home button </t>
+  </si>
+  <si>
+    <t>Get animations working in app</t>
+  </si>
+  <si>
+    <t>Create an quit/exit button</t>
+  </si>
+  <si>
+    <t>Write an exit method</t>
+  </si>
+  <si>
+    <t>Write method to attach buttons to opening an animation</t>
+  </si>
+  <si>
+    <t>Find multiple lottie animations to use from the internet</t>
+  </si>
+  <si>
+    <t>Write method to return to home screen</t>
+  </si>
+  <si>
+    <t>Create an app to open(start xamarin project in VS)</t>
   </si>
 </sst>
 </file>
@@ -230,9 +278,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -413,8 +464,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B8:G16" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
-  <autoFilter ref="B8:G16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B8:G17" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
+  <autoFilter ref="B8:G17"/>
   <tableColumns count="6">
     <tableColumn id="1" name="UserStory#" dataDxfId="46"/>
     <tableColumn id="6" name="StoryName" dataDxfId="45"/>
@@ -428,8 +479,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B4:H13" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
-  <autoFilter ref="B4:H13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B4:H16" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
+  <autoFilter ref="B4:H16"/>
   <sortState ref="B5:H13">
     <sortCondition descending="1" ref="B19:B28"/>
   </sortState>
@@ -790,7 +841,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="3:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="6" t="s">
         <v>0</v>
       </c>
       <c r="E3" t="s">
@@ -798,75 +849,75 @@
       </c>
     </row>
     <row r="4" spans="3:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
     </row>
     <row r="12" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -882,7 +933,7 @@
   <dimension ref="B7:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -897,7 +948,7 @@
   </cols>
   <sheetData>
     <row r="7" spans="2:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -926,16 +977,16 @@
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -943,16 +994,16 @@
         <v>2</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -960,16 +1011,16 @@
         <v>3</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -977,36 +1028,53 @@
         <v>4</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="F12" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="3">
+        <v>5</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="2">
+        <v>6</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="2">
-        <v>5</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1031,10 +1099,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:H13"/>
+  <dimension ref="B3:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C14" sqref="C14:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1047,7 +1115,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="2"/>
@@ -1089,13 +1157,15 @@
       <c r="C5" s="2">
         <v>1</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>16</v>
+      <c r="D5" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="2"/>
+        <v>42</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="G5" s="2" t="s">
         <v>19</v>
       </c>
@@ -1106,86 +1176,175 @@
         <v>3</v>
       </c>
       <c r="C6" s="2">
-        <v>3</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="2">
-        <v>2</v>
-      </c>
-      <c r="C7" s="2">
-        <v>2</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3">
+        <v>3</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8" s="2">
         <v>4</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="D8" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="C9" s="2">
+        <v>5</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3">
+        <v>6</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3">
+        <v>7</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="C12" s="2">
+        <v>8</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="C13" s="2">
+        <v>9</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="2">
+        <v>2</v>
+      </c>
+      <c r="C14" s="2">
+        <v>10</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1200,7 +1359,7 @@
   <dimension ref="B2:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1211,7 +1370,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1237,55 +1396,61 @@
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
-        <v>10</v>
-      </c>
-      <c r="C4" s="2">
         <v>1</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G4" s="2"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
-        <v>3</v>
-      </c>
-      <c r="C5" s="2">
-        <v>3</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="C5" s="3">
+        <v>8</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
-        <v>2</v>
-      </c>
-      <c r="C6" s="2">
-        <v>2</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="C6" s="3">
+        <v>9</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
-      <c r="C7" s="2">
-        <v>4</v>
-      </c>
+      <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -1342,154 +1507,154 @@
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1507,7 +1672,7 @@
   <dimension ref="B2:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1518,7 +1683,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1544,18 +1709,20 @@
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
-        <v>10</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="C4" s="3">
+        <v>4</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="G4" s="2" t="s">
         <v>19</v>
       </c>
@@ -1564,54 +1731,70 @@
       <c r="B5" s="2">
         <v>3</v>
       </c>
-      <c r="C5" s="2">
-        <v>3</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="C5" s="3">
+        <v>5</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
-        <v>2</v>
-      </c>
-      <c r="C6" s="2">
-        <v>2</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="C6" s="3">
+        <v>6</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2">
-        <v>4</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="B7" s="2">
+        <v>3</v>
+      </c>
+      <c r="C7" s="3">
+        <v>7</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
@@ -1649,154 +1832,154 @@
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1814,7 +1997,7 @@
   <dimension ref="B2:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1825,7 +2008,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1851,18 +2034,20 @@
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
-        <v>10</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="G4" s="2" t="s">
         <v>19</v>
       </c>
@@ -1871,35 +2056,41 @@
       <c r="B5" s="2">
         <v>3</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="3">
         <v>3</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="D5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
-        <v>2</v>
-      </c>
-      <c r="C6" s="2">
-        <v>2</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="C6" s="3">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
-      <c r="C7" s="2">
-        <v>4</v>
-      </c>
+      <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -1956,154 +2147,154 @@
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2132,7 +2323,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2268,154 +2459,154 @@
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
adds finished excel doc
</commit_message>
<xml_diff>
--- a/final+project.xlsx
+++ b/final+project.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Project Description" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="66">
   <si>
     <t>Your Name:</t>
   </si>
@@ -65,9 +65,6 @@
     <t>Link to Branch:</t>
   </si>
   <si>
-    <t>Bug</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -80,18 +77,9 @@
     <t>StoryName</t>
   </si>
   <si>
-    <t>LoadModel</t>
-  </si>
-  <si>
-    <t>SeeInstructions</t>
-  </si>
-  <si>
     <t>BacklogId</t>
   </si>
   <si>
-    <t>someClass.cs</t>
-  </si>
-  <si>
     <t>InSprint</t>
   </si>
   <si>
@@ -122,9 +110,6 @@
     <t xml:space="preserve">AFTER SHIPPING, REVIEW MAIN BACKLOG AND MARK STATUS </t>
   </si>
   <si>
-    <t>I plan on doing a 2D Xamarin app. I think that 3D would be pushing my comfort zone the most, however I feel that a portfolio piece that shows the ability to publish to multiple platforms is the most relevant in our smartphone driven world. Probably with the inclusion of Lottie examples.</t>
-  </si>
-  <si>
     <t>Will Fergus</t>
   </si>
   <si>
@@ -188,9 +173,6 @@
     <t>To exit the app</t>
   </si>
   <si>
-    <t>Make sure xamarin is working properly</t>
-  </si>
-  <si>
     <t>UI_Selection</t>
   </si>
   <si>
@@ -219,13 +201,63 @@
   </si>
   <si>
     <t>Create an app to open(start xamarin project in VS)</t>
+  </si>
+  <si>
+    <t>Make sure app opens in WinForms</t>
+  </si>
+  <si>
+    <t>Make sure app opens in iOS</t>
+  </si>
+  <si>
+    <t>Make sure xamarin is working properly in various OS</t>
+  </si>
+  <si>
+    <t>Tailor UI specifically for the various OS</t>
+  </si>
+  <si>
+    <t>Customize UI specifically for iOS</t>
+  </si>
+  <si>
+    <t>Customize UI specifically for WinForms</t>
+  </si>
+  <si>
+    <t>Customize UI specifically for Android</t>
+  </si>
+  <si>
+    <t>Make sure app opens in Android</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">I plan on doing a cross platform 2D Xamarin app with the inclusion of multiple Lottie examples. Hopefully with </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>some</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> customization specific to the various OS.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,6 +284,14 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -845,7 +885,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="3:8" ht="23.25" x14ac:dyDescent="0.35">
@@ -855,7 +895,7 @@
     </row>
     <row r="5" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C5" s="8" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
@@ -932,7 +972,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B7:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -957,7 +997,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>3</v>
@@ -977,16 +1017,16 @@
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -994,16 +1034,16 @@
         <v>2</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1011,16 +1051,16 @@
         <v>3</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1028,16 +1068,16 @@
         <v>4</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1045,16 +1085,16 @@
         <v>5</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="G13" s="3"/>
     </row>
@@ -1063,16 +1103,16 @@
         <v>6</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1102,7 +1142,7 @@
   <dimension ref="B3:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14:F14"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1121,7 +1161,7 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -1129,25 +1169,25 @@
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="H4" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1158,156 +1198,186 @@
         <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="2"/>
+        <v>56</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" s="2">
         <v>2</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="H6" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="3"/>
+      <c r="B7" s="3">
+        <v>4</v>
+      </c>
       <c r="C7" s="3">
         <v>3</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+      <c r="H7" s="3">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
+      <c r="B8" s="2">
+        <v>4</v>
+      </c>
       <c r="C8" s="2">
         <v>4</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="H8" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
+      <c r="B9" s="2">
+        <v>4</v>
+      </c>
       <c r="C9" s="2">
         <v>5</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
+      <c r="H9" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
+      <c r="B10" s="3">
+        <v>4</v>
+      </c>
       <c r="C10" s="3">
         <v>6</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+      <c r="H10" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
+      <c r="B11" s="3">
+        <v>4</v>
+      </c>
       <c r="C11" s="3">
         <v>7</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
+      <c r="H11" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="2"/>
+      <c r="B12" s="2">
+        <v>6</v>
+      </c>
       <c r="C12" s="2">
         <v>8</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
+      <c r="H12" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
+      <c r="B13" s="2">
+        <v>6</v>
+      </c>
       <c r="C13" s="2">
         <v>9</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
+      <c r="H13" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
@@ -1317,25 +1387,39 @@
         <v>10</v>
       </c>
       <c r="D14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="F14" s="2" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
+      <c r="H14" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="B15" s="2">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2">
+        <v>11</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
+      <c r="H15" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
@@ -1371,27 +1455,27 @@
   <sheetData>
     <row r="2" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
@@ -1402,13 +1486,13 @@
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="G4" s="2"/>
     </row>
@@ -1420,13 +1504,13 @@
         <v>8</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="G5" s="2"/>
     </row>
@@ -1438,13 +1522,13 @@
         <v>9</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="G6" s="2"/>
     </row>
@@ -1503,7 +1587,7 @@
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
@@ -1672,7 +1756,7 @@
   <dimension ref="B2:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1684,27 +1768,27 @@
   <sheetData>
     <row r="2" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
@@ -1715,17 +1799,15 @@
         <v>4</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>19</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="G4" s="2"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
@@ -1735,13 +1817,13 @@
         <v>5</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="G5" s="2"/>
     </row>
@@ -1753,13 +1835,13 @@
         <v>6</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="G6" s="2"/>
     </row>
@@ -1771,13 +1853,13 @@
         <v>7</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G7" s="2"/>
     </row>
@@ -1828,7 +1910,7 @@
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
@@ -1997,7 +2079,7 @@
   <dimension ref="B2:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2009,27 +2091,27 @@
   <sheetData>
     <row r="2" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
@@ -2040,17 +2122,15 @@
         <v>2</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>19</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="G4" s="2"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
@@ -2060,48 +2140,68 @@
         <v>3</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="3">
         <v>10</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="F6" s="3" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="B7" s="2">
+        <v>3</v>
+      </c>
+      <c r="C7" s="3">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="B8" s="2">
+        <v>3</v>
+      </c>
+      <c r="C8" s="3">
+        <v>10</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -2143,7 +2243,7 @@
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
@@ -2311,8 +2411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2324,80 +2424,86 @@
   <sheetData>
     <row r="2" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2" t="s">
-        <v>19</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" s="2"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C5" s="2">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C6" s="2">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
-      <c r="C7" s="2">
-        <v>4</v>
-      </c>
+      <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -2450,12 +2556,12 @@
     </row>
     <row r="16" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
adds sprint 1 & 2 updates
</commit_message>
<xml_diff>
--- a/final+project.xlsx
+++ b/final+project.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Project Description" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="72">
   <si>
     <t>Your Name:</t>
   </si>
@@ -252,12 +252,30 @@
       <t xml:space="preserve"> customization specific to the various OS.</t>
     </r>
   </si>
+  <si>
+    <t>complete</t>
+  </si>
+  <si>
+    <t>Started a visual studio xamarin project and found a couple of animations that I can work with. I have had no success getting them to work yet, predicting a difficulty as 5 may have been optimistic of me. Also the reason I put 'getting an animation working'  in sprit 1 and as a high priority. It is the largest barrior and the whole point.</t>
+  </si>
+  <si>
+    <t>https://github.com/wfergus/GraphicsAppsFinal/tree/sprint-1#graphicsappsfinal</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>sprint 1-&gt;2 (incomplete)</t>
+  </si>
+  <si>
+    <t>incomplete (moved to sprint 2)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -297,6 +315,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -315,10 +341,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -338,8 +365,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="49">
@@ -538,8 +573,26 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="B3:G12" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="B3:G12" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="B3:G12"/>
+  <sortState ref="B4:H12">
+    <sortCondition descending="1" ref="B19:B28"/>
+  </sortState>
+  <tableColumns count="6">
+    <tableColumn id="12" name="Points" dataDxfId="5"/>
+    <tableColumn id="10" name="BacklogId" dataDxfId="4"/>
+    <tableColumn id="1" name="StoryName" dataDxfId="3"/>
+    <tableColumn id="2" name="BacklogType" dataDxfId="2"/>
+    <tableColumn id="3" name="Description" dataDxfId="1"/>
+    <tableColumn id="4" name="In" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table245" displayName="Table245" ref="B3:G13" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+  <autoFilter ref="B3:G13"/>
   <sortState ref="B4:H12">
     <sortCondition descending="1" ref="B19:B28"/>
   </sortState>
@@ -555,8 +608,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table245" displayName="Table245" ref="B3:G12" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table246" displayName="Table246" ref="B3:G12" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="B3:G12"/>
   <sortState ref="B4:H12">
     <sortCondition descending="1" ref="B19:B28"/>
@@ -573,8 +626,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table246" displayName="Table246" ref="B3:G12" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table247" displayName="Table247" ref="B3:G12" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="B3:G12"/>
   <sortState ref="B4:H12">
     <sortCondition descending="1" ref="B19:B28"/>
@@ -586,24 +639,6 @@
     <tableColumn id="2" name="BacklogType" dataDxfId="10"/>
     <tableColumn id="3" name="Description" dataDxfId="9"/>
     <tableColumn id="4" name="In" dataDxfId="8"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table247" displayName="Table247" ref="B3:G12" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="B3:G12"/>
-  <sortState ref="B4:H12">
-    <sortCondition descending="1" ref="B19:B28"/>
-  </sortState>
-  <tableColumns count="6">
-    <tableColumn id="12" name="Points" dataDxfId="5"/>
-    <tableColumn id="10" name="BacklogId" dataDxfId="4"/>
-    <tableColumn id="1" name="StoryName" dataDxfId="3"/>
-    <tableColumn id="2" name="BacklogType" dataDxfId="2"/>
-    <tableColumn id="3" name="Description" dataDxfId="1"/>
-    <tableColumn id="4" name="In" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -875,7 +910,7 @@
   <dimension ref="C3:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:H12"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1142,7 +1177,7 @@
   <dimension ref="B3:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1206,7 +1241,9 @@
       <c r="F5" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="H5" s="2">
         <v>1</v>
       </c>
@@ -1353,7 +1390,9 @@
       <c r="F12" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="H12" s="2">
         <v>1</v>
       </c>
@@ -1374,7 +1413,9 @@
       <c r="F13" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G13" s="2"/>
+      <c r="G13" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="H13" s="2">
         <v>1</v>
       </c>
@@ -1442,15 +1483,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="27.5703125" customWidth="1"/>
     <col min="6" max="6" width="71.42578125" customWidth="1"/>
-    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="7" max="7" width="29.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
@@ -1494,7 +1535,9 @@
       <c r="F4" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="G4" s="2"/>
+      <c r="G4" s="2" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
@@ -1512,7 +1555,9 @@
       <c r="F5" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
@@ -1530,7 +1575,9 @@
       <c r="F6" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
@@ -1584,6 +1631,9 @@
       <c r="B15" t="s">
         <v>10</v>
       </c>
+      <c r="D15" s="11" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
@@ -1591,172 +1641,178 @@
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
+      <c r="B19" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B19:I33"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D15" r:id="rId1" location="graphicsappsfinal"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I33"/>
+  <dimension ref="B2:I34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1792,29 +1848,31 @@
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
-        <v>3</v>
-      </c>
-      <c r="C4" s="3">
-        <v>4</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="B4" s="7">
+        <v>7</v>
+      </c>
+      <c r="C4" s="7">
+        <v>9</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G4" s="2"/>
+      <c r="F4" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>3</v>
       </c>
       <c r="C5" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>47</v>
@@ -1823,7 +1881,7 @@
         <v>37</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="G5" s="2"/>
     </row>
@@ -1832,16 +1890,16 @@
         <v>3</v>
       </c>
       <c r="C6" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>37</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G6" s="2"/>
     </row>
@@ -1850,7 +1908,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>41</v>
@@ -1859,16 +1917,26 @@
         <v>37</v>
       </c>
       <c r="F7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
+        <v>3</v>
+      </c>
+      <c r="C8" s="3">
+        <v>7</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -1881,10 +1949,10 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
@@ -1903,23 +1971,23 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
     </row>
@@ -2063,10 +2131,15 @@
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
     </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B19:I33"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -2247,154 +2320,154 @@
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2411,7 +2484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -2565,154 +2638,154 @@
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>